<commit_message>
[CSV] IdolStatType Enum 생성
</commit_message>
<xml_diff>
--- a/Design/Tables/Enum.xlsx
+++ b/Design/Tables/Enum.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20343"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEDA0B2-2C42-4EB4-B2B2-D8F53B4EADE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFE6193-77C9-4FB2-BDB7-6B0D8B8AED31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,25 +20,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>ThemeType</t>
-  </si>
-  <si>
-    <t>Empty</t>
-  </si>
-  <si>
-    <t>Tree</t>
-  </si>
-  <si>
-    <t>Flower</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>IdolStatType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sexy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beauty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vocal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>humor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>intelligen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF666666"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +88,20 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,8 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -356,13 +407,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -391,6 +445,46 @@
       </c>
       <c r="B4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>